<commit_message>
Better filtering for TEST and ERROR results
</commit_message>
<xml_diff>
--- a/data/n1-pXRF.xlsx
+++ b/data/n1-pXRF.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">Sample</t>
   </si>
@@ -83,9 +83,6 @@
     <t xml:space="preserve">Ag</t>
   </si>
   <si>
-    <t xml:space="preserve">Sn</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ba</t>
   </si>
   <si>
@@ -336,9 +333,6 @@
   </si>
   <si>
     <t xml:space="preserve">RLZ_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST %</t>
   </si>
   <si>
     <t xml:space="preserve">TI-1</t>
@@ -773,13 +767,10 @@
       <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="n">
         <v>0.130675270799723</v>
@@ -811,7 +802,7 @@
         <v>0.302704194260486</v>
       </c>
       <c r="M2" t="n">
-        <v>0.52406836100093</v>
+        <v>0.521862762461381</v>
       </c>
       <c r="N2" t="n">
         <v>0.291666666666667</v>
@@ -824,7 +815,7 @@
       </c>
       <c r="Q2"/>
       <c r="R2" t="n">
-        <v>0.436507936507936</v>
+        <v>0.509259259259259</v>
       </c>
       <c r="S2" t="n">
         <v>0.028657616892911</v>
@@ -836,16 +827,15 @@
         <v>0.284615384615385</v>
       </c>
       <c r="V2" t="n">
-        <v>0.0108695652173913</v>
+        <v>0.181818181818182</v>
       </c>
       <c r="W2"/>
       <c r="X2"/>
       <c r="Y2"/>
-      <c r="Z2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="n">
         <v>0.173115498536102</v>
@@ -879,7 +869,7 @@
         <v>0.202262693156733</v>
       </c>
       <c r="M3" t="n">
-        <v>0.408765486508986</v>
+        <v>0.406025542633371</v>
       </c>
       <c r="N3" t="n">
         <v>0.25</v>
@@ -892,7 +882,7 @@
       </c>
       <c r="Q3"/>
       <c r="R3" t="n">
-        <v>0.293650793650794</v>
+        <v>0.342592592592593</v>
       </c>
       <c r="S3" t="n">
         <v>0.0380844645550528</v>
@@ -907,11 +897,10 @@
       <c r="W3"/>
       <c r="X3"/>
       <c r="Y3"/>
-      <c r="Z3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="n">
         <v>0.211070139048936</v>
@@ -943,7 +932,7 @@
         <v>0.211368653421634</v>
       </c>
       <c r="M4" t="n">
-        <v>0.397463395524215</v>
+        <v>0.394671074640376</v>
       </c>
       <c r="N4" t="n">
         <v>0.229166666666667</v>
@@ -956,7 +945,7 @@
       </c>
       <c r="Q4"/>
       <c r="R4" t="n">
-        <v>0.222222222222222</v>
+        <v>0.259259259259259</v>
       </c>
       <c r="S4" t="n">
         <v>0.0222473604826546</v>
@@ -971,11 +960,10 @@
       <c r="W4"/>
       <c r="X4"/>
       <c r="Y4"/>
-      <c r="Z4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="n">
         <v>0.141024984422081</v>
@@ -1007,7 +995,7 @@
         <v>0.185706401766004</v>
       </c>
       <c r="M5" t="n">
-        <v>0.413211889721365</v>
+        <v>0.410492551705138</v>
       </c>
       <c r="N5" t="n">
         <v>0.145833333333333</v>
@@ -1020,7 +1008,7 @@
       </c>
       <c r="Q5"/>
       <c r="R5" t="n">
-        <v>0.246031746031746</v>
+        <v>0.287037037037037</v>
       </c>
       <c r="S5" t="n">
         <v>0.0173453996983409</v>
@@ -1035,11 +1023,10 @@
       <c r="W5"/>
       <c r="X5"/>
       <c r="Y5"/>
-      <c r="Z5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="n">
         <v>0.207335706298601</v>
@@ -1071,7 +1058,7 @@
         <v>0.207229580573951</v>
       </c>
       <c r="M6" t="n">
-        <v>0.508496155917928</v>
+        <v>0.506218391483165</v>
       </c>
       <c r="N6" t="n">
         <v>0.3125</v>
@@ -1084,7 +1071,7 @@
       </c>
       <c r="Q6"/>
       <c r="R6" t="n">
-        <v>0.293650793650794</v>
+        <v>0.342592592592593</v>
       </c>
       <c r="S6" t="n">
         <v>0.0107466063348416</v>
@@ -1099,11 +1086,10 @@
       <c r="W6"/>
       <c r="X6"/>
       <c r="Y6"/>
-      <c r="Z6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
         <v>0.193298507080484</v>
@@ -1137,7 +1123,7 @@
         <v>0.313465783664459</v>
       </c>
       <c r="M7" t="n">
-        <v>0.621957788551001</v>
+        <v>0.620205836629474</v>
       </c>
       <c r="N7" t="n">
         <v>0.229166666666667</v>
@@ -1150,7 +1136,7 @@
       </c>
       <c r="Q7"/>
       <c r="R7" t="n">
-        <v>0.317460317460317</v>
+        <v>0.37037037037037</v>
       </c>
       <c r="S7" t="n">
         <v>0.0450603318250377</v>
@@ -1162,16 +1148,15 @@
         <v>0.420512820512821</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0072463768115942</v>
+        <v>0.121212121212121</v>
       </c>
       <c r="W7"/>
       <c r="X7"/>
       <c r="Y7"/>
-      <c r="Z7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="n">
         <v>0.17719563306104</v>
@@ -1203,7 +1188,7 @@
         <v>0.193708609271523</v>
       </c>
       <c r="M8" t="n">
-        <v>0.470995543802948</v>
+        <v>0.468543991184053</v>
       </c>
       <c r="N8" t="n">
         <v>0.34375</v>
@@ -1218,7 +1203,7 @@
         <v>0.0666666666666667</v>
       </c>
       <c r="R8" t="n">
-        <v>0.428571428571428</v>
+        <v>0.5</v>
       </c>
       <c r="S8" t="n">
         <v>0.0258295625942685</v>
@@ -1233,11 +1218,10 @@
       <c r="W8"/>
       <c r="X8"/>
       <c r="Y8"/>
-      <c r="Z8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" t="n">
         <v>0.198573660085529</v>
@@ -1271,7 +1255,7 @@
         <v>0.251931567328918</v>
       </c>
       <c r="M9" t="n">
-        <v>0.499730669408942</v>
+        <v>0.497412283291025</v>
       </c>
       <c r="N9" t="n">
         <v>0.34375</v>
@@ -1286,7 +1270,7 @@
         <v>0.15</v>
       </c>
       <c r="R9" t="n">
-        <v>0.412698412698413</v>
+        <v>0.481481481481481</v>
       </c>
       <c r="S9" t="n">
         <v>0.0303544494720965</v>
@@ -1301,11 +1285,10 @@
       <c r="W9"/>
       <c r="X9"/>
       <c r="Y9"/>
-      <c r="Z9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
         <v>0.315164784512561</v>
@@ -1339,7 +1322,7 @@
         <v>0.44757174392936</v>
       </c>
       <c r="M10" t="n">
-        <v>0.862621810880956</v>
+        <v>0.861985162445638</v>
       </c>
       <c r="N10" t="n">
         <v>0.447916666666667</v>
@@ -1354,7 +1337,7 @@
         <v>0.1</v>
       </c>
       <c r="R10" t="n">
-        <v>0.5</v>
+        <v>0.583333333333333</v>
       </c>
       <c r="S10" t="n">
         <v>0.0256410256410256</v>
@@ -1366,16 +1349,15 @@
         <v>0.405128205128205</v>
       </c>
       <c r="V10" t="n">
-        <v>0.0235507246376812</v>
+        <v>0.393939393939394</v>
       </c>
       <c r="W10"/>
       <c r="X10"/>
       <c r="Y10"/>
-      <c r="Z10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="n">
         <v>0.261589545295468</v>
@@ -1409,7 +1391,7 @@
         <v>0.260761589403974</v>
       </c>
       <c r="M11" t="n">
-        <v>0.578414377356643</v>
+        <v>0.576460633252652</v>
       </c>
       <c r="N11" t="n">
         <v>0.239583333333333</v>
@@ -1422,7 +1404,7 @@
       </c>
       <c r="Q11"/>
       <c r="R11" t="n">
-        <v>0.404761904761905</v>
+        <v>0.472222222222222</v>
       </c>
       <c r="S11" t="n">
         <v>0.0411010558069382</v>
@@ -1434,16 +1416,15 @@
         <v>0.503846153846154</v>
       </c>
       <c r="V11" t="n">
-        <v>0.0072463768115942</v>
+        <v>0.121212121212121</v>
       </c>
       <c r="W11"/>
       <c r="X11"/>
       <c r="Y11"/>
-      <c r="Z11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" t="n">
         <v>0.128579720536393</v>
@@ -1475,7 +1456,7 @@
         <v>0.18901766004415</v>
       </c>
       <c r="M12" t="n">
-        <v>0.324440526908575</v>
+        <v>0.321309797902277</v>
       </c>
       <c r="N12" t="n">
         <v>0.28125</v>
@@ -1488,7 +1469,7 @@
       </c>
       <c r="Q12"/>
       <c r="R12" t="n">
-        <v>0.238095238095238</v>
+        <v>0.277777777777778</v>
       </c>
       <c r="S12" t="n">
         <v>0.00226244343891403</v>
@@ -1503,11 +1484,10 @@
       <c r="W12"/>
       <c r="X12"/>
       <c r="Y12"/>
-      <c r="Z12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="n">
         <v>0.171749763130266</v>
@@ -1539,7 +1519,7 @@
         <v>0.188741721854305</v>
       </c>
       <c r="M13" t="n">
-        <v>0.33037559375153</v>
+        <v>0.327272369482653</v>
       </c>
       <c r="N13" t="n">
         <v>0.0833333333333333</v>
@@ -1554,7 +1534,7 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="R13" t="n">
-        <v>0.206349206349206</v>
+        <v>0.240740740740741</v>
       </c>
       <c r="S13" t="n">
         <v>0.00207390648567119</v>
@@ -1569,11 +1549,10 @@
       <c r="W13"/>
       <c r="X13"/>
       <c r="Y13"/>
-      <c r="Z13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" t="n">
         <v>0.210579327887463</v>
@@ -1607,7 +1586,7 @@
         <v>0.2530353200883</v>
       </c>
       <c r="M14" t="n">
-        <v>0.435189265951716</v>
+        <v>0.432571777161186</v>
       </c>
       <c r="N14" t="n">
         <v>0.28125</v>
@@ -1622,7 +1601,7 @@
         <v>0.0666666666666667</v>
       </c>
       <c r="R14" t="n">
-        <v>0.301587301587302</v>
+        <v>0.351851851851852</v>
       </c>
       <c r="S14" t="n">
         <v>0.0271493212669683</v>
@@ -1637,11 +1616,10 @@
       <c r="W14"/>
       <c r="X14"/>
       <c r="Y14"/>
-      <c r="Z14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" t="n">
         <v>0.0793022799245431</v>
@@ -1675,7 +1653,7 @@
         <v>0.218818984547461</v>
       </c>
       <c r="M15" t="n">
-        <v>0.443190832966064</v>
+        <v>0.440610425644961</v>
       </c>
       <c r="N15" t="n">
         <v>0.28125</v>
@@ -1688,7 +1666,7 @@
       </c>
       <c r="Q15"/>
       <c r="R15" t="n">
-        <v>0.388888888888889</v>
+        <v>0.453703703703704</v>
       </c>
       <c r="S15" t="n">
         <v>0.026395173453997</v>
@@ -1700,16 +1678,15 @@
         <v>0.437179487179487</v>
       </c>
       <c r="V15" t="n">
-        <v>0.016304347826087</v>
+        <v>0.272727272727273</v>
       </c>
       <c r="W15"/>
       <c r="X15"/>
       <c r="Y15"/>
-      <c r="Z15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" t="n">
         <v>0.0967708893498246</v>
@@ -1745,7 +1722,7 @@
         <v>0.360651214128035</v>
       </c>
       <c r="M16" t="n">
-        <v>0.471896577053034</v>
+        <v>0.469449200070842</v>
       </c>
       <c r="N16" t="n">
         <v>0.34375</v>
@@ -1760,7 +1737,7 @@
         <v>0.2</v>
       </c>
       <c r="R16" t="n">
-        <v>0.285714285714286</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="S16" t="n">
         <v>0.0228129713423831</v>
@@ -1772,16 +1749,15 @@
         <v>0.28974358974359</v>
       </c>
       <c r="V16" t="n">
-        <v>0.0126811594202899</v>
+        <v>0.212121212121212</v>
       </c>
       <c r="W16"/>
       <c r="X16"/>
       <c r="Y16"/>
-      <c r="Z16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" t="n">
         <v>0.136326001041373</v>
@@ -1815,7 +1791,7 @@
         <v>0.217991169977925</v>
       </c>
       <c r="M17" t="n">
-        <v>0.37857107879144</v>
+        <v>0.37569120569888</v>
       </c>
       <c r="N17" t="n">
         <v>0.40625</v>
@@ -1828,7 +1804,7 @@
       </c>
       <c r="Q17"/>
       <c r="R17" t="n">
-        <v>0.380952380952381</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="S17" t="n">
         <v>0.0231900452488688</v>
@@ -1841,11 +1817,10 @@
       <c r="W17"/>
       <c r="X17"/>
       <c r="Y17"/>
-      <c r="Z17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="n">
         <v>0.187861172995997</v>
@@ -1877,7 +1852,7 @@
         <v>0.332505518763797</v>
       </c>
       <c r="M18" t="n">
-        <v>0.470368738063758</v>
+        <v>0.467914280654112</v>
       </c>
       <c r="N18" t="n">
         <v>0.302083333333333</v>
@@ -1892,7 +1867,7 @@
         <v>0.25</v>
       </c>
       <c r="R18" t="n">
-        <v>0.333333333333333</v>
+        <v>0.388888888888889</v>
       </c>
       <c r="S18" t="n">
         <v>0.02526395173454</v>
@@ -1907,11 +1882,10 @@
       <c r="W18"/>
       <c r="X18"/>
       <c r="Y18"/>
-      <c r="Z18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" t="n">
         <v>0.167271644772221</v>
@@ -1943,7 +1917,7 @@
         <v>0.240273178807947</v>
       </c>
       <c r="M19" t="n">
-        <v>0.406757749375643</v>
+        <v>0.404008501092154</v>
       </c>
       <c r="N19" t="n">
         <v>0.2890625</v>
@@ -1956,7 +1930,7 @@
       </c>
       <c r="Q19"/>
       <c r="R19" t="n">
-        <v>0.410714285714286</v>
+        <v>0.479166666666667</v>
       </c>
       <c r="S19" t="n">
         <v>0.0202205882352941</v>
@@ -1971,11 +1945,10 @@
       <c r="W19"/>
       <c r="X19"/>
       <c r="Y19"/>
-      <c r="Z19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" t="n">
         <v>0.272489821003303</v>
@@ -2007,7 +1980,7 @@
         <v>0.383278145695364</v>
       </c>
       <c r="M20" t="n">
-        <v>0.782841192889672</v>
+        <v>0.781834819056615</v>
       </c>
       <c r="N20" t="n">
         <v>0.333333333333333</v>
@@ -2022,7 +1995,7 @@
         <v>0.15</v>
       </c>
       <c r="R20" t="n">
-        <v>0.484126984126984</v>
+        <v>0.564814814814815</v>
       </c>
       <c r="S20" t="n">
         <v>0.027526395173454</v>
@@ -2034,18 +2007,17 @@
         <v>0.420512820512821</v>
       </c>
       <c r="V20" t="n">
-        <v>0.0217391304347826</v>
+        <v>0.363636363636364</v>
       </c>
       <c r="W20"/>
-      <c r="X20"/>
-      <c r="Y20" t="n">
-        <v>0.0721601489757914</v>
-      </c>
-      <c r="Z20"/>
+      <c r="X20" t="n">
+        <v>0.193508114856429</v>
+      </c>
+      <c r="Y20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="n">
         <v>0.239912763650952</v>
@@ -2079,7 +2051,7 @@
         <v>0.310430463576159</v>
       </c>
       <c r="M21" t="n">
-        <v>0.677136281279075</v>
+        <v>0.675640041718323</v>
       </c>
       <c r="N21" t="n">
         <v>0.270833333333333</v>
@@ -2094,7 +2066,7 @@
         <v>0.183333333333333</v>
       </c>
       <c r="R21" t="n">
-        <v>0.484126984126984</v>
+        <v>0.564814814814815</v>
       </c>
       <c r="S21" t="n">
         <v>0.0269607843137255</v>
@@ -2106,16 +2078,15 @@
         <v>0.521794871794872</v>
       </c>
       <c r="V21" t="n">
-        <v>0.0126811594202899</v>
+        <v>0.212121212121212</v>
       </c>
       <c r="W21"/>
       <c r="X21"/>
       <c r="Y21"/>
-      <c r="Z21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" t="n">
         <v>0.209149573634478</v>
@@ -2149,7 +2120,7 @@
         <v>0.344922737306843</v>
       </c>
       <c r="M22" t="n">
-        <v>0.733264776455609</v>
+        <v>0.732028651829112</v>
       </c>
       <c r="N22" t="n">
         <v>0.34375</v>
@@ -2164,7 +2135,7 @@
         <v>0.15</v>
       </c>
       <c r="R22" t="n">
-        <v>0.476190476190476</v>
+        <v>0.555555555555555</v>
       </c>
       <c r="S22" t="n">
         <v>0.0235671191553544</v>
@@ -2176,16 +2147,15 @@
         <v>0.511538461538461</v>
       </c>
       <c r="V22" t="n">
-        <v>0.0181159420289855</v>
+        <v>0.303030303030303</v>
       </c>
       <c r="W22"/>
       <c r="X22"/>
       <c r="Y22"/>
-      <c r="Z22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" t="n">
         <v>0.176841395440151</v>
@@ -2217,7 +2187,7 @@
         <v>0.274282560706402</v>
       </c>
       <c r="M23" t="n">
-        <v>0.419617060868714</v>
+        <v>0.41692740618297</v>
       </c>
       <c r="N23" t="n">
         <v>0.28125</v>
@@ -2230,7 +2200,7 @@
       </c>
       <c r="Q23"/>
       <c r="R23" t="n">
-        <v>0.23015873015873</v>
+        <v>0.268518518518518</v>
       </c>
       <c r="S23" t="n">
         <v>0.00622171945701358</v>
@@ -2245,11 +2215,10 @@
       <c r="W23"/>
       <c r="X23"/>
       <c r="Y23"/>
-      <c r="Z23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" t="n">
         <v>0.172778332607786</v>
@@ -2281,7 +2250,7 @@
         <v>0.211368653421634</v>
       </c>
       <c r="M24" t="n">
-        <v>0.391097399735566</v>
+        <v>0.388275577070665</v>
       </c>
       <c r="N24" t="n">
         <v>0.3125</v>
@@ -2294,7 +2263,7 @@
       </c>
       <c r="Q24"/>
       <c r="R24" t="n">
-        <v>0.285714285714286</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="S24" t="n">
         <v>0.01263197586727</v>
@@ -2309,11 +2278,10 @@
       <c r="W24"/>
       <c r="X24"/>
       <c r="Y24"/>
-      <c r="Z24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" t="n">
         <v>0.145954435652523</v>
@@ -2345,7 +2313,7 @@
         <v>0.123620309050773</v>
       </c>
       <c r="M25" t="n">
-        <v>0.282140933352921</v>
+        <v>0.278814176358305</v>
       </c>
       <c r="N25"/>
       <c r="O25" t="n">
@@ -2358,7 +2326,7 @@
         <v>0.133333333333333</v>
       </c>
       <c r="R25" t="n">
-        <v>0.277777777777778</v>
+        <v>0.324074074074074</v>
       </c>
       <c r="S25" t="n">
         <v>0.0158371040723982</v>
@@ -2373,11 +2341,10 @@
       <c r="W25"/>
       <c r="X25"/>
       <c r="Y25"/>
-      <c r="Z25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" t="n">
         <v>0.179696636022978</v>
@@ -2411,7 +2378,7 @@
         <v>0.27924944812362</v>
       </c>
       <c r="M26" t="n">
-        <v>0.525145683365163</v>
+        <v>0.522945077434717</v>
       </c>
       <c r="N26" t="n">
         <v>0.3125</v>
@@ -2424,7 +2391,7 @@
       </c>
       <c r="Q26"/>
       <c r="R26" t="n">
-        <v>0.420634920634921</v>
+        <v>0.490740740740741</v>
       </c>
       <c r="S26" t="n">
         <v>0.0228129713423831</v>
@@ -2436,16 +2403,15 @@
         <v>0.423076923076923</v>
       </c>
       <c r="V26" t="n">
-        <v>0.0326086956521739</v>
+        <v>0.545454545454546</v>
       </c>
       <c r="W26"/>
       <c r="X26"/>
       <c r="Y26"/>
-      <c r="Z26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" t="n">
         <v>0.105917048645788</v>
@@ -2477,7 +2443,7 @@
         <v>0.279525386313466</v>
       </c>
       <c r="M27" t="n">
-        <v>0.477067724401352</v>
+        <v>0.474644311942854</v>
       </c>
       <c r="N27" t="n">
         <v>0.25</v>
@@ -2490,7 +2456,7 @@
       </c>
       <c r="Q27"/>
       <c r="R27" t="n">
-        <v>0.412698412698413</v>
+        <v>0.481481481481481</v>
       </c>
       <c r="S27" t="n">
         <v>0.0258295625942685</v>
@@ -2505,11 +2471,10 @@
       <c r="W27"/>
       <c r="X27"/>
       <c r="Y27"/>
-      <c r="Z27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" t="n">
         <v>0.171685744283117</v>
@@ -2541,7 +2506,7 @@
         <v>0.240066225165563</v>
       </c>
       <c r="M28" t="n">
-        <v>0.360501444591352</v>
+        <v>0.357537831827932</v>
       </c>
       <c r="N28" t="n">
         <v>0.364583333333333</v>
@@ -2556,7 +2521,7 @@
         <v>0.116666666666667</v>
       </c>
       <c r="R28" t="n">
-        <v>0.23015873015873</v>
+        <v>0.268518518518518</v>
       </c>
       <c r="S28" t="n">
         <v>0.0360105580693816</v>
@@ -2571,11 +2536,10 @@
       <c r="W28"/>
       <c r="X28"/>
       <c r="Y28"/>
-      <c r="Z28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" t="n">
         <v>0.204262801635468</v>
@@ -2609,7 +2573,7 @@
         <v>0.222682119205298</v>
       </c>
       <c r="M29" t="n">
-        <v>0.400754125654963</v>
+        <v>0.397977054922565</v>
       </c>
       <c r="N29" t="n">
         <v>0.15625</v>
@@ -2622,7 +2586,7 @@
       </c>
       <c r="Q29"/>
       <c r="R29" t="n">
-        <v>0.238095238095238</v>
+        <v>0.277777777777778</v>
       </c>
       <c r="S29" t="n">
         <v>0.0109351432880845</v>
@@ -2637,11 +2601,10 @@
       <c r="W29"/>
       <c r="X29"/>
       <c r="Y29"/>
-      <c r="Z29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" t="n">
         <v>0.104226951081065</v>
@@ -2673,7 +2636,7 @@
         <v>0.331401766004415</v>
       </c>
       <c r="M30" t="n">
-        <v>0.475628029969149</v>
+        <v>0.473197945569396</v>
       </c>
       <c r="N30" t="n">
         <v>0.333333333333333</v>
@@ -2686,7 +2649,7 @@
       </c>
       <c r="Q30"/>
       <c r="R30" t="n">
-        <v>0.412698412698413</v>
+        <v>0.481481481481481</v>
       </c>
       <c r="S30" t="n">
         <v>0.0288461538461538</v>
@@ -2701,11 +2664,10 @@
       <c r="W30"/>
       <c r="X30"/>
       <c r="Y30"/>
-      <c r="Z30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" t="n">
         <v>0.245076950654273</v>
@@ -2737,7 +2699,7 @@
         <v>0.257174392935982</v>
       </c>
       <c r="M31" t="n">
-        <v>0.567151461730571</v>
+        <v>0.565145522167778</v>
       </c>
       <c r="N31" t="n">
         <v>0.208333333333333</v>
@@ -2752,7 +2714,7 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="R31" t="n">
-        <v>0.341269841269841</v>
+        <v>0.398148148148148</v>
       </c>
       <c r="S31" t="n">
         <v>0.0180995475113122</v>
@@ -2764,16 +2726,15 @@
         <v>0.353846153846154</v>
       </c>
       <c r="V31" t="n">
-        <v>0.0181159420289855</v>
+        <v>0.303030303030303</v>
       </c>
       <c r="W31"/>
       <c r="X31"/>
       <c r="Y31"/>
-      <c r="Z31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" t="n">
         <v>0.194916049951772</v>
@@ -2807,7 +2768,7 @@
         <v>0.31401766004415</v>
       </c>
       <c r="M32" t="n">
-        <v>0.566867440380001</v>
+        <v>0.564860184583899</v>
       </c>
       <c r="N32" t="n">
         <v>0.260416666666667</v>
@@ -2822,7 +2783,7 @@
         <v>0.15</v>
       </c>
       <c r="R32" t="n">
-        <v>0.349206349206349</v>
+        <v>0.407407407407407</v>
       </c>
       <c r="S32" t="n">
         <v>0.0497737556561086</v>
@@ -2834,16 +2795,15 @@
         <v>0.361538461538462</v>
       </c>
       <c r="V32" t="n">
-        <v>0.0108695652173913</v>
+        <v>0.181818181818182</v>
       </c>
       <c r="W32"/>
       <c r="X32"/>
       <c r="Y32"/>
-      <c r="Z32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" t="n">
         <v>0.164869871023363</v>
@@ -2877,7 +2837,7 @@
         <v>0.204470198675497</v>
       </c>
       <c r="M33" t="n">
-        <v>0.428774300964693</v>
+        <v>0.426127083456324</v>
       </c>
       <c r="N33" t="n">
         <v>0.208333333333333</v>
@@ -2890,7 +2850,7 @@
       </c>
       <c r="Q33"/>
       <c r="R33" t="n">
-        <v>0.301587301587302</v>
+        <v>0.351851851851852</v>
       </c>
       <c r="S33" t="n">
         <v>0.0254524886877828</v>
@@ -2905,11 +2865,10 @@
       <c r="W33"/>
       <c r="X33"/>
       <c r="Y33"/>
-      <c r="Z33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" t="n">
         <v>0.0977866550579157</v>
@@ -2943,7 +2902,7 @@
         <v>0.170805739514349</v>
       </c>
       <c r="M34" t="n">
-        <v>0.32536114783801</v>
+        <v>0.322234685243127</v>
       </c>
       <c r="N34" t="n">
         <v>0.239583333333333</v>
@@ -2956,7 +2915,7 @@
       </c>
       <c r="Q34"/>
       <c r="R34" t="n">
-        <v>0.317460317460317</v>
+        <v>0.37037037037037</v>
       </c>
       <c r="S34" t="n">
         <v>0.0322398190045249</v>
@@ -2969,11 +2928,10 @@
       <c r="W34"/>
       <c r="X34"/>
       <c r="Y34"/>
-      <c r="Z34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" t="n">
         <v>0.227305318685821</v>
@@ -3007,7 +2965,7 @@
         <v>0.230132450331126</v>
       </c>
       <c r="M35" t="n">
-        <v>0.436237206796925</v>
+        <v>0.433624574453431</v>
       </c>
       <c r="N35" t="n">
         <v>0.1875</v>
@@ -3020,7 +2978,7 @@
       </c>
       <c r="Q35"/>
       <c r="R35" t="n">
-        <v>0.293650793650794</v>
+        <v>0.342592592592593</v>
       </c>
       <c r="S35" t="n">
         <v>0.0143288084464555</v>
@@ -3035,11 +2993,10 @@
       <c r="W35"/>
       <c r="X35"/>
       <c r="Y35"/>
-      <c r="Z35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" t="n">
         <v>0.241598593292532</v>
@@ -3071,7 +3028,7 @@
         <v>0.238686534216336</v>
       </c>
       <c r="M36" t="n">
-        <v>0.421859850154253</v>
+        <v>0.419180589172915</v>
       </c>
       <c r="N36" t="n">
         <v>0.270833333333333</v>
@@ -3084,7 +3041,7 @@
       </c>
       <c r="Q36"/>
       <c r="R36" t="n">
-        <v>0.333333333333333</v>
+        <v>0.388888888888889</v>
       </c>
       <c r="S36" t="n">
         <v>0.0164027149321267</v>
@@ -3099,11 +3056,10 @@
       <c r="W36"/>
       <c r="X36"/>
       <c r="Y36"/>
-      <c r="Z36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" t="n">
         <v>0.224966496803326</v>
@@ -3137,7 +3093,7 @@
         <v>0.275110375275938</v>
       </c>
       <c r="M37" t="n">
-        <v>0.532089515694628</v>
+        <v>0.529921089399217</v>
       </c>
       <c r="N37" t="n">
         <v>0.166666666666667</v>
@@ -3152,7 +3108,7 @@
         <v>0.0333333333333333</v>
       </c>
       <c r="R37" t="n">
-        <v>0.293650793650794</v>
+        <v>0.342592592592593</v>
       </c>
       <c r="S37" t="n">
         <v>0.0196078431372549</v>
@@ -3164,16 +3120,15 @@
         <v>0.291025641025641</v>
       </c>
       <c r="V37" t="n">
-        <v>0.0072463768115942</v>
+        <v>0.121212121212121</v>
       </c>
       <c r="W37"/>
       <c r="X37"/>
       <c r="Y37"/>
-      <c r="Z37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" t="n">
         <v>0.110445315100766</v>
@@ -3205,7 +3160,7 @@
         <v>0.213024282560706</v>
       </c>
       <c r="M38" t="n">
-        <v>0.393741736447774</v>
+        <v>0.390932168368853</v>
       </c>
       <c r="N38" t="n">
         <v>0.364583333333333</v>
@@ -3220,7 +3175,7 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="R38" t="n">
-        <v>0.357142857142857</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="S38" t="n">
         <v>0.0292232277526395</v>
@@ -3235,11 +3190,10 @@
       <c r="W38"/>
       <c r="X38"/>
       <c r="Y38"/>
-      <c r="Z38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" t="n">
         <v>0.194625831178032</v>
@@ -3273,7 +3227,7 @@
         <v>0.309602649006623</v>
       </c>
       <c r="M39" t="n">
-        <v>0.591058224376867</v>
+        <v>0.589163075348801</v>
       </c>
       <c r="N39" t="n">
         <v>0.1875</v>
@@ -3288,7 +3242,7 @@
         <v>0.1</v>
       </c>
       <c r="R39" t="n">
-        <v>0.317460317460317</v>
+        <v>0.37037037037037</v>
       </c>
       <c r="S39" t="n">
         <v>0.0318627450980392</v>
@@ -3300,16 +3254,15 @@
         <v>0.332051282051282</v>
       </c>
       <c r="V39" t="n">
-        <v>0.0108695652173913</v>
+        <v>0.181818181818182</v>
       </c>
       <c r="W39"/>
       <c r="X39"/>
       <c r="Y39"/>
-      <c r="Z39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" t="n">
         <v>0.190485945729089</v>
@@ -3341,7 +3294,7 @@
         <v>0.377483443708609</v>
       </c>
       <c r="M40" t="n">
-        <v>0.711561627736154</v>
+        <v>0.710224924729913</v>
       </c>
       <c r="N40" t="n">
         <v>0.46875</v>
@@ -3354,7 +3307,7 @@
       </c>
       <c r="Q40"/>
       <c r="R40" t="n">
-        <v>0.531746031746032</v>
+        <v>0.62037037037037</v>
       </c>
       <c r="S40" t="n">
         <v>0.0348793363499246</v>
@@ -3366,16 +3319,15 @@
         <v>0.593589743589744</v>
       </c>
       <c r="V40" t="n">
-        <v>0.0344202898550725</v>
+        <v>0.575757575757576</v>
       </c>
       <c r="W40"/>
       <c r="X40"/>
       <c r="Y40"/>
-      <c r="Z40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41" t="n">
         <v>0.14944132886055</v>
@@ -3409,7 +3361,7 @@
         <v>0.353752759381898</v>
       </c>
       <c r="M41" t="n">
-        <v>0.656118701336859</v>
+        <v>0.654525060511246</v>
       </c>
       <c r="N41" t="n">
         <v>0.333333333333333</v>
@@ -3424,7 +3376,7 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="R41" t="n">
-        <v>0.380952380952381</v>
+        <v>0.444444444444444</v>
       </c>
       <c r="S41" t="n">
         <v>0.029788838612368</v>
@@ -3439,11 +3391,10 @@
       <c r="W41"/>
       <c r="X41"/>
       <c r="Y41"/>
-      <c r="Z41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B42" t="n">
         <v>0.140871339188924</v>
@@ -3475,7 +3426,7 @@
         <v>0.308222958057395</v>
       </c>
       <c r="M42" t="n">
-        <v>0.516380196856177</v>
+        <v>0.514138969242576</v>
       </c>
       <c r="N42" t="n">
         <v>0.260416666666667</v>
@@ -3490,7 +3441,7 @@
         <v>0.3</v>
       </c>
       <c r="R42" t="n">
-        <v>0.341269841269841</v>
+        <v>0.398148148148148</v>
       </c>
       <c r="S42" t="n">
         <v>0.0367647058823529</v>
@@ -3505,11 +3456,10 @@
       <c r="W42"/>
       <c r="X42"/>
       <c r="Y42"/>
-      <c r="Z42"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B43" t="n">
         <v>0.146091009193106</v>
@@ -3541,7 +3491,7 @@
         <v>0.22378587196468</v>
       </c>
       <c r="M43" t="n">
-        <v>0.395671122863719</v>
+        <v>0.392870496093827</v>
       </c>
       <c r="N43" t="n">
         <v>0.21875</v>
@@ -3554,7 +3504,7 @@
       </c>
       <c r="Q43"/>
       <c r="R43" t="n">
-        <v>0.277777777777778</v>
+        <v>0.324074074074074</v>
       </c>
       <c r="S43" t="n">
         <v>0.0194193061840121</v>
@@ -3569,11 +3519,10 @@
       <c r="W43"/>
       <c r="X43"/>
       <c r="Y43"/>
-      <c r="Z43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" t="n">
         <v>0.130542965182283</v>
@@ -3605,7 +3554,7 @@
         <v>0.359823399558499</v>
       </c>
       <c r="M44" t="n">
-        <v>0.556133392096371</v>
+        <v>0.554076391758663</v>
       </c>
       <c r="N44" t="n">
         <v>0.395833333333333</v>
@@ -3618,7 +3567,7 @@
       </c>
       <c r="Q44"/>
       <c r="R44" t="n">
-        <v>0.531746031746032</v>
+        <v>0.62037037037037</v>
       </c>
       <c r="S44" t="n">
         <v>0.0311085972850679</v>
@@ -3630,16 +3579,15 @@
         <v>0.338461538461538</v>
       </c>
       <c r="V44" t="n">
-        <v>0.0235507246376812</v>
+        <v>0.393939393939394</v>
       </c>
       <c r="W44"/>
       <c r="X44"/>
       <c r="Y44"/>
-      <c r="Z44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" t="n">
         <v>0.234488233335894</v>
@@ -3671,7 +3619,7 @@
         <v>0.283388520971302</v>
       </c>
       <c r="M45" t="n">
-        <v>0.532931785906665</v>
+        <v>0.530767262923825</v>
       </c>
       <c r="N45" t="n">
         <v>0.15625</v>
@@ -3684,7 +3632,7 @@
       </c>
       <c r="Q45"/>
       <c r="R45" t="n">
-        <v>0.301587301587302</v>
+        <v>0.351851851851852</v>
       </c>
       <c r="S45" t="n">
         <v>0.0367647058823529</v>
@@ -3697,15 +3645,14 @@
       </c>
       <c r="V45"/>
       <c r="W45"/>
-      <c r="X45"/>
-      <c r="Y45" t="n">
-        <v>0.0689013035381751</v>
-      </c>
-      <c r="Z45"/>
+      <c r="X45" t="n">
+        <v>0.184769038701623</v>
+      </c>
+      <c r="Y45"/>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" t="n">
         <v>0.239938371189812</v>
@@ -3739,7 +3686,7 @@
         <v>0.168598233995585</v>
       </c>
       <c r="M46" t="n">
-        <v>0.313608540228196</v>
+        <v>0.310427612806738</v>
       </c>
       <c r="N46" t="n">
         <v>0.239583333333333</v>
@@ -3754,7 +3701,7 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="R46" t="n">
-        <v>0.293650793650794</v>
+        <v>0.342592592592593</v>
       </c>
       <c r="S46" t="n">
         <v>0.189856711915535</v>
@@ -3767,11 +3714,10 @@
       <c r="W46"/>
       <c r="X46"/>
       <c r="Y46"/>
-      <c r="Z46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" t="n">
         <v>0.211718863366708</v>
@@ -3803,7 +3749,7 @@
         <v>0.192604856512141</v>
       </c>
       <c r="M47" t="n">
-        <v>0.413192302042016</v>
+        <v>0.410472873251077</v>
       </c>
       <c r="N47" t="n">
         <v>0.09375</v>
@@ -3818,7 +3764,7 @@
         <v>0.133333333333333</v>
       </c>
       <c r="R47" t="n">
-        <v>0.412698412698413</v>
+        <v>0.481481481481481</v>
       </c>
       <c r="S47" t="n">
         <v>0.0818250377073906</v>
@@ -3832,14 +3778,13 @@
       <c r="V47"/>
       <c r="W47"/>
       <c r="X47"/>
-      <c r="Y47"/>
-      <c r="Z47" t="n">
-        <v>0.468992248062015</v>
+      <c r="Y47" t="n">
+        <v>0.677871148459384</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" t="n">
         <v>0.14393570800577</v>
@@ -3873,7 +3818,7 @@
         <v>0.188741721854305</v>
       </c>
       <c r="M48" t="n">
-        <v>0.784868517702365</v>
+        <v>0.783871539051892</v>
       </c>
       <c r="N48" t="n">
         <v>0.166666666666667</v>
@@ -3888,7 +3833,7 @@
         <v>0.616666666666667</v>
       </c>
       <c r="R48" t="n">
-        <v>0.309523809523809</v>
+        <v>0.361111111111111</v>
       </c>
       <c r="S48" t="n">
         <v>0.069947209653092</v>
@@ -3902,14 +3847,13 @@
       <c r="V48"/>
       <c r="W48"/>
       <c r="X48"/>
-      <c r="Y48"/>
-      <c r="Z48" t="n">
-        <v>0.544573643410853</v>
+      <c r="Y48" t="n">
+        <v>0.787114845938375</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B49" t="n">
         <v>0.152113048748218</v>
@@ -3943,7 +3887,7 @@
         <v>0.230132450331126</v>
       </c>
       <c r="M49" t="n">
-        <v>0.544145732334362</v>
+        <v>0.542033177873546</v>
       </c>
       <c r="N49" t="n">
         <v>0.333333333333333</v>
@@ -3958,7 +3902,7 @@
         <v>0.283333333333333</v>
       </c>
       <c r="R49" t="n">
-        <v>0.468253968253968</v>
+        <v>0.546296296296296</v>
       </c>
       <c r="S49" t="n">
         <v>0.0716440422322775</v>
@@ -3972,14 +3916,13 @@
       <c r="V49"/>
       <c r="W49"/>
       <c r="X49"/>
-      <c r="Y49"/>
-      <c r="Z49" t="n">
-        <v>0.397286821705426</v>
+      <c r="Y49" t="n">
+        <v>0.574229691876751</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50" t="n">
         <v>0.10443181139194</v>
@@ -4011,7 +3954,7 @@
         <v>0.197847682119205</v>
       </c>
       <c r="M50" t="n">
-        <v>0.403878360511238</v>
+        <v>0.401115768345239</v>
       </c>
       <c r="N50" t="n">
         <v>0.375</v>
@@ -4024,7 +3967,7 @@
       </c>
       <c r="Q50"/>
       <c r="R50" t="n">
-        <v>0.357142857142857</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="S50" t="n">
         <v>0.0341251885369532</v>
@@ -4039,11 +3982,10 @@
       <c r="W50"/>
       <c r="X50"/>
       <c r="Y50"/>
-      <c r="Z50"/>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51"/>
       <c r="C51" t="n">
@@ -4075,7 +4017,7 @@
         <v>0.473233995584989</v>
       </c>
       <c r="M51" t="n">
-        <v>0.897164683414132</v>
+        <v>0.896688116181593</v>
       </c>
       <c r="N51" t="n">
         <v>0.614583333333333</v>
@@ -4090,7 +4032,7 @@
         <v>0.633333333333333</v>
       </c>
       <c r="R51" t="n">
-        <v>0.373015873015873</v>
+        <v>0.435185185185185</v>
       </c>
       <c r="S51" t="n">
         <v>0.154034690799397</v>
@@ -4102,22 +4044,21 @@
         <v>0.846153846153846</v>
       </c>
       <c r="V51" t="n">
-        <v>0.0181159420289855</v>
+        <v>0.303030303030303</v>
       </c>
       <c r="W51" t="n">
-        <v>0.0168612191958495</v>
-      </c>
-      <c r="X51"/>
+        <v>0.206349206349206</v>
+      </c>
+      <c r="X51" t="n">
+        <v>0.371410736579276</v>
+      </c>
       <c r="Y51" t="n">
-        <v>0.138500931098696</v>
-      </c>
-      <c r="Z51" t="n">
-        <v>0.467054263565891</v>
+        <v>0.675070028011205</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" t="n">
         <v>0.170866303039615</v>
@@ -4149,7 +4090,7 @@
         <v>0.181015452538631</v>
       </c>
       <c r="M52" t="n">
-        <v>0.359394740708095</v>
+        <v>0.356425999173505</v>
       </c>
       <c r="N52" t="n">
         <v>0.21875</v>
@@ -4175,11 +4116,10 @@
       <c r="W52"/>
       <c r="X52"/>
       <c r="Y52"/>
-      <c r="Z52"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" t="n">
         <v>0.327102165544203</v>
@@ -4213,7 +4153,7 @@
         <v>0.209437086092715</v>
       </c>
       <c r="M53" t="n">
-        <v>0.404152588022134</v>
+        <v>0.401391266702088</v>
       </c>
       <c r="N53" t="n">
         <v>0.4375</v>
@@ -4226,7 +4166,7 @@
       </c>
       <c r="Q53"/>
       <c r="R53" t="n">
-        <v>0.277777777777778</v>
+        <v>0.324074074074074</v>
       </c>
       <c r="S53" t="n">
         <v>0.407051282051282</v>
@@ -4239,11 +4179,10 @@
       <c r="W53"/>
       <c r="X53"/>
       <c r="Y53"/>
-      <c r="Z53"/>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54" t="n">
         <v>0.370792894761551</v>
@@ -4279,7 +4218,7 @@
         <v>0.172185430463576</v>
       </c>
       <c r="M54" t="n">
-        <v>0.385005631457813</v>
+        <v>0.382155577857804</v>
       </c>
       <c r="N54" t="n">
         <v>0.270833333333333</v>
@@ -4292,7 +4231,7 @@
       </c>
       <c r="Q54"/>
       <c r="R54" t="n">
-        <v>0.222222222222222</v>
+        <v>0.259259259259259</v>
       </c>
       <c r="S54" t="n">
         <v>0.562217194570136</v>
@@ -4305,11 +4244,10 @@
       <c r="W54"/>
       <c r="X54"/>
       <c r="Y54"/>
-      <c r="Z54"/>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" t="n">
         <v>0.123556374996799</v>
@@ -4341,7 +4279,7 @@
         <v>0.187637969094923</v>
       </c>
       <c r="M55" t="n">
-        <v>0.322334851378483</v>
+        <v>0.319194364090757</v>
       </c>
       <c r="N55" t="n">
         <v>0.375</v>
@@ -4354,7 +4292,7 @@
       </c>
       <c r="Q55"/>
       <c r="R55" t="n">
-        <v>0.420634920634921</v>
+        <v>0.490740740740741</v>
       </c>
       <c r="S55" t="n">
         <v>0.0669306184012066</v>
@@ -4367,11 +4305,10 @@
       <c r="W55"/>
       <c r="X55"/>
       <c r="Y55"/>
-      <c r="Z55"/>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" t="n">
         <v>0.154993896869905</v>
@@ -4405,7 +4342,7 @@
         <v>0.301324503311258</v>
       </c>
       <c r="M56" t="n">
-        <v>0.411733019930464</v>
+        <v>0.409006828423559</v>
       </c>
       <c r="N56" t="n">
         <v>0.40625</v>
@@ -4420,7 +4357,7 @@
         <v>0.1</v>
       </c>
       <c r="R56" t="n">
-        <v>0.436507936507936</v>
+        <v>0.509259259259259</v>
       </c>
       <c r="S56" t="n">
         <v>0.0757918552036199</v>
@@ -4432,16 +4369,15 @@
         <v>0.507692307692308</v>
       </c>
       <c r="V56" t="n">
-        <v>0.0289855072463768</v>
+        <v>0.484848484848485</v>
       </c>
       <c r="W56"/>
       <c r="X56"/>
       <c r="Y56"/>
-      <c r="Z56"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57" t="n">
         <v>0.346918132698266</v>
@@ -4473,7 +4409,7 @@
         <v>0.15424944812362</v>
       </c>
       <c r="M57" t="n">
-        <v>0.142617893345086</v>
+        <v>0.138644548084303</v>
       </c>
       <c r="N57"/>
       <c r="O57" t="n">
@@ -4484,7 +4420,7 @@
       </c>
       <c r="Q57"/>
       <c r="R57" t="n">
-        <v>0.166666666666667</v>
+        <v>0.194444444444444</v>
       </c>
       <c r="S57" t="n">
         <v>0.39762443438914</v>
@@ -4495,15 +4431,14 @@
       </c>
       <c r="V57"/>
       <c r="W57"/>
-      <c r="X57"/>
-      <c r="Y57" t="n">
-        <v>0.192970204841713</v>
-      </c>
-      <c r="Z57"/>
+      <c r="X57" t="n">
+        <v>0.517478152309613</v>
+      </c>
+      <c r="Y57"/>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" t="n">
         <v>0.324251192884519</v>
@@ -4535,7 +4470,7 @@
         <v>0.251931567328918</v>
       </c>
       <c r="M58" t="n">
-        <v>0.323294647666618</v>
+        <v>0.320158608339729</v>
       </c>
       <c r="N58" t="n">
         <v>0.34375</v>
@@ -4559,11 +4494,10 @@
       <c r="W58"/>
       <c r="X58"/>
       <c r="Y58"/>
-      <c r="Z58"/>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B59" t="n">
         <v>0.208039913617236</v>
@@ -4597,7 +4531,7 @@
         <v>0.359823399558499</v>
       </c>
       <c r="M59" t="n">
-        <v>0.40881445570736</v>
+        <v>0.406074738768522</v>
       </c>
       <c r="N59" t="n">
         <v>0.708333333333333</v>
@@ -4610,7 +4544,7 @@
       </c>
       <c r="Q59"/>
       <c r="R59" t="n">
-        <v>0.626984126984127</v>
+        <v>0.731481481481481</v>
       </c>
       <c r="S59" t="n">
         <v>0.151018099547511</v>
@@ -4620,16 +4554,15 @@
         <v>0.86025641025641</v>
       </c>
       <c r="V59" t="n">
-        <v>0.0380434782608696</v>
+        <v>0.636363636363636</v>
       </c>
       <c r="W59"/>
       <c r="X59"/>
       <c r="Y59"/>
-      <c r="Z59"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B60" t="n">
         <v>0.325757769754082</v>
@@ -4663,7 +4596,7 @@
         <v>0.525386313465784</v>
       </c>
       <c r="M60" t="n">
-        <v>0.504088928064248</v>
+        <v>0.501790739319519</v>
       </c>
       <c r="N60" t="n">
         <v>0.666666666666667</v>
@@ -4678,7 +4611,7 @@
         <v>0.0666666666666667</v>
       </c>
       <c r="R60" t="n">
-        <v>0.563492063492063</v>
+        <v>0.657407407407407</v>
       </c>
       <c r="S60" t="n">
         <v>0.143665158371041</v>
@@ -4690,18 +4623,17 @@
         <v>0.775641025641026</v>
       </c>
       <c r="V60" t="n">
-        <v>0.0561594202898551</v>
+        <v>0.939393939393939</v>
       </c>
       <c r="W60"/>
-      <c r="X60"/>
-      <c r="Y60" t="n">
-        <v>0.0989292364990689</v>
-      </c>
-      <c r="Z60"/>
+      <c r="X60" t="n">
+        <v>0.265293383270911</v>
+      </c>
+      <c r="Y60"/>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B61" t="n">
         <v>0.207899072153509</v>
@@ -4737,7 +4669,7 @@
         <v>0.252207505518764</v>
       </c>
       <c r="M61" t="n">
-        <v>0.388541207580432</v>
+        <v>0.385707538815751</v>
       </c>
       <c r="N61"/>
       <c r="O61" t="n">
@@ -4748,7 +4680,7 @@
       </c>
       <c r="Q61"/>
       <c r="R61" t="n">
-        <v>0.531746031746032</v>
+        <v>0.62037037037037</v>
       </c>
       <c r="S61" t="n">
         <v>0.10369532428356</v>
@@ -4761,11 +4693,10 @@
       <c r="W61"/>
       <c r="X61"/>
       <c r="Y61"/>
-      <c r="Z61"/>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" t="n">
         <v>0.328472168873183</v>
@@ -4797,7 +4728,7 @@
         <v>0.222958057395144</v>
       </c>
       <c r="M62" t="n">
-        <v>0.417452622300573</v>
+        <v>0.414752937009269</v>
       </c>
       <c r="N62"/>
       <c r="O62" t="n">
@@ -4808,7 +4739,7 @@
       </c>
       <c r="Q62"/>
       <c r="R62" t="n">
-        <v>0.388888888888889</v>
+        <v>0.453703703703704</v>
       </c>
       <c r="S62" t="n">
         <v>0.105580693815988</v>
@@ -4820,16 +4751,15 @@
         <v>0.58974358974359</v>
       </c>
       <c r="V62" t="n">
-        <v>0.0289855072463768</v>
+        <v>0.484848484848485</v>
       </c>
       <c r="W62"/>
       <c r="X62"/>
       <c r="Y62"/>
-      <c r="Z62"/>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63" t="n">
         <v>0.606540165424701</v>
@@ -4861,7 +4791,7 @@
         <v>0.0747792494481236</v>
       </c>
       <c r="M63" t="n">
-        <v>0.13356838548553</v>
+        <v>0.129553102308283</v>
       </c>
       <c r="N63"/>
       <c r="O63" t="n">
@@ -4872,7 +4802,7 @@
       </c>
       <c r="Q63"/>
       <c r="R63" t="n">
-        <v>0.0317460317460317</v>
+        <v>0.037037037037037</v>
       </c>
       <c r="S63" t="n">
         <v>0.900829562594268</v>
@@ -4885,11 +4815,10 @@
       <c r="W63"/>
       <c r="X63"/>
       <c r="Y63"/>
-      <c r="Z63"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B64" t="n">
         <v>0.374245644584432</v>
@@ -4921,7 +4850,7 @@
         <v>0.0767108167770419</v>
       </c>
       <c r="M64" t="n">
-        <v>0.0913079672885755</v>
+        <v>0.0870968376724325</v>
       </c>
       <c r="N64"/>
       <c r="O64" t="n">
@@ -4943,11 +4872,10 @@
       <c r="W64"/>
       <c r="X64"/>
       <c r="Y64"/>
-      <c r="Z64"/>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B65" t="n">
         <v>0.413198979112784</v>
@@ -4981,7 +4909,7 @@
         <v>0.259105960264901</v>
       </c>
       <c r="M65" t="n">
-        <v>0.33888644042897</v>
+        <v>0.335822657772005</v>
       </c>
       <c r="N65"/>
       <c r="O65" t="n">
@@ -4992,7 +4920,7 @@
       </c>
       <c r="Q65"/>
       <c r="R65" t="n">
-        <v>0.0873015873015873</v>
+        <v>0.101851851851852</v>
       </c>
       <c r="S65" t="n">
         <v>0.849547511312217</v>
@@ -5005,11 +4933,10 @@
       <c r="W65"/>
       <c r="X65"/>
       <c r="Y65"/>
-      <c r="Z65"/>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B66" t="n">
         <v>0.443625003200942</v>
@@ -5043,7 +4970,7 @@
         <v>0.175496688741722</v>
       </c>
       <c r="M66" t="n">
-        <v>0.234268645022281</v>
+        <v>0.230720034634079</v>
       </c>
       <c r="N66"/>
       <c r="O66" t="n">
@@ -5065,11 +4992,10 @@
       <c r="W66"/>
       <c r="X66"/>
       <c r="Y66"/>
-      <c r="Z66"/>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B67" t="n">
         <v>0.38883767381117</v>
@@ -5101,7 +5027,7 @@
         <v>0.0607064017660044</v>
       </c>
       <c r="M67" t="n">
-        <v>0.0716909064198619</v>
+        <v>0.0673888659306925</v>
       </c>
       <c r="N67"/>
       <c r="O67" t="n">
@@ -5123,11 +5049,10 @@
       <c r="W67"/>
       <c r="X67"/>
       <c r="Y67"/>
-      <c r="Z67"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B68" t="n">
         <v>0.301204407911022</v>
@@ -5159,7 +5084,7 @@
         <v>0.331401766004415</v>
       </c>
       <c r="M68" t="n">
-        <v>0.151628225845943</v>
+        <v>0.147696636952201</v>
       </c>
       <c r="N68" t="n">
         <v>0.385416666666667</v>
@@ -5172,7 +5097,7 @@
       </c>
       <c r="Q68"/>
       <c r="R68" t="n">
-        <v>0.174603174603175</v>
+        <v>0.203703703703704</v>
       </c>
       <c r="S68" t="n">
         <v>0.473981900452489</v>
@@ -5185,11 +5110,10 @@
       <c r="W68"/>
       <c r="X68"/>
       <c r="Y68"/>
-      <c r="Z68"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B69" t="n">
         <v>0.382060211859705</v>
@@ -5221,7 +5145,7 @@
         <v>0.4969646799117</v>
       </c>
       <c r="M69" t="n">
-        <v>0.192821115518339</v>
+        <v>0.189080425841746</v>
       </c>
       <c r="N69" t="n">
         <v>0.104166666666667</v>
@@ -5234,7 +5158,7 @@
       </c>
       <c r="Q69"/>
       <c r="R69" t="n">
-        <v>0.142857142857143</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="S69" t="n">
         <v>0.507918552036199</v>
@@ -5245,15 +5169,14 @@
       </c>
       <c r="V69"/>
       <c r="W69"/>
-      <c r="X69"/>
-      <c r="Y69" t="n">
-        <v>0.21415270018622</v>
-      </c>
-      <c r="Z69"/>
+      <c r="X69" t="n">
+        <v>0.574282147315855</v>
+      </c>
+      <c r="Y69"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B70" t="n">
         <v>0.229563050028595</v>
@@ -5285,7 +5208,7 @@
         <v>0.231236203090508</v>
       </c>
       <c r="M70" t="n">
-        <v>0.394936584888105</v>
+        <v>0.392132554066553</v>
       </c>
       <c r="N70" t="n">
         <v>0.5625</v>
@@ -5298,7 +5221,7 @@
       </c>
       <c r="Q70"/>
       <c r="R70" t="n">
-        <v>0.595238095238095</v>
+        <v>0.694444444444444</v>
       </c>
       <c r="S70" t="n">
         <v>0.126885369532428</v>
@@ -5313,11 +5236,10 @@
       <c r="W70"/>
       <c r="X70"/>
       <c r="Y70"/>
-      <c r="Z70"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B71" t="n">
         <v>0.302403694314273</v>
@@ -5349,7 +5271,7 @@
         <v>0.322847682119205</v>
       </c>
       <c r="M71" t="n">
-        <v>0.47496204887126</v>
+        <v>0.472528878131334</v>
       </c>
       <c r="N71" t="n">
         <v>0.822916666666667</v>
@@ -5362,7 +5284,7 @@
       </c>
       <c r="Q71"/>
       <c r="R71" t="n">
-        <v>0.634920634920635</v>
+        <v>0.740740740740741</v>
       </c>
       <c r="S71" t="n">
         <v>0.112933634992459</v>
@@ -5372,16 +5294,15 @@
         <v>0.643589743589744</v>
       </c>
       <c r="V71" t="n">
-        <v>0.0434782608695652</v>
+        <v>0.727272727272727</v>
       </c>
       <c r="W71"/>
       <c r="X71"/>
       <c r="Y71"/>
-      <c r="Z71"/>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B72" t="n">
         <v>0.181105050660248</v>
@@ -5415,7 +5336,7 @@
         <v>0.164183222958057</v>
       </c>
       <c r="M72" t="n">
-        <v>0.305753880808971</v>
+        <v>0.302536552728418</v>
       </c>
       <c r="N72" t="n">
         <v>0.177083333333333</v>
@@ -5430,7 +5351,7 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="R72" t="n">
-        <v>0.261904761904762</v>
+        <v>0.305555555555556</v>
       </c>
       <c r="S72" t="n">
         <v>0.0116892911010558</v>
@@ -5445,11 +5366,10 @@
       <c r="W72"/>
       <c r="X72"/>
       <c r="Y72"/>
-      <c r="Z72"/>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B73" t="n">
         <v>0.216460525978848</v>
@@ -5481,7 +5401,7 @@
         <v>0.365618101545254</v>
       </c>
       <c r="M73" t="n">
-        <v>0.316047206307233</v>
+        <v>0.312877580337289</v>
       </c>
       <c r="N73" t="n">
         <v>0.260416666666667</v>
@@ -5494,7 +5414,7 @@
       </c>
       <c r="Q73"/>
       <c r="R73" t="n">
-        <v>0.317460317460317</v>
+        <v>0.37037037037037</v>
       </c>
       <c r="S73" t="n">
         <v>0.00867269984917044</v>
@@ -5509,11 +5429,10 @@
       <c r="W73"/>
       <c r="X73"/>
       <c r="Y73"/>
-      <c r="Z73"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B74" t="n">
         <v>0.17139979343252</v>
@@ -5545,7 +5464,7 @@
         <v>0.225441501103753</v>
       </c>
       <c r="M74" t="n">
-        <v>0.4188825228931</v>
+        <v>0.416189464155696</v>
       </c>
       <c r="N74" t="n">
         <v>0.15625</v>
@@ -5558,7 +5477,7 @@
       </c>
       <c r="Q74"/>
       <c r="R74" t="n">
-        <v>0.261904761904762</v>
+        <v>0.305555555555556</v>
       </c>
       <c r="S74" t="n">
         <v>0.0213046757164404</v>
@@ -5573,11 +5492,10 @@
       <c r="W74"/>
       <c r="X74"/>
       <c r="Y74"/>
-      <c r="Z74"/>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B75" t="n">
         <v>0.455724565312028</v>
@@ -5611,7 +5529,7 @@
         <v>0.31705298013245</v>
       </c>
       <c r="M75" t="n">
-        <v>0.324469908427599</v>
+        <v>0.321339315583368</v>
       </c>
       <c r="N75"/>
       <c r="O75" t="n">
@@ -5633,11 +5551,10 @@
       <c r="W75"/>
       <c r="X75"/>
       <c r="Y75"/>
-      <c r="Z75"/>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B76" t="n">
         <v>0.482194224646402</v>
@@ -5671,7 +5588,7 @@
         <v>0.266832229580574</v>
       </c>
       <c r="M76" t="n">
-        <v>0.360511238431027</v>
+        <v>0.357547671054962</v>
       </c>
       <c r="N76"/>
       <c r="O76" t="n">
@@ -5693,11 +5610,10 @@
       <c r="W76"/>
       <c r="X76"/>
       <c r="Y76"/>
-      <c r="Z76"/>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B77"/>
       <c r="C77" t="n">
@@ -5727,7 +5643,7 @@
         <v>0.198399558498896</v>
       </c>
       <c r="M77" t="n">
-        <v>0.345565839087214</v>
+        <v>0.342533010606687</v>
       </c>
       <c r="N77" t="n">
         <v>0.25</v>
@@ -5740,7 +5656,7 @@
       </c>
       <c r="Q77"/>
       <c r="R77" t="n">
-        <v>0.309523809523809</v>
+        <v>0.361111111111111</v>
       </c>
       <c r="S77" t="n">
         <v>0.040158371040724</v>
@@ -5755,11 +5671,10 @@
       <c r="W77"/>
       <c r="X77"/>
       <c r="Y77"/>
-      <c r="Z77"/>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B78" t="n">
         <v>0.210664686350328</v>
@@ -5793,7 +5708,7 @@
         <v>0.466887417218543</v>
       </c>
       <c r="M78" t="n">
-        <v>0.744850888790951</v>
+        <v>0.743668457405986</v>
       </c>
       <c r="N78" t="n">
         <v>0.302083333333333</v>
@@ -5808,7 +5723,7 @@
         <v>0.133333333333333</v>
       </c>
       <c r="R78" t="n">
-        <v>0.452380952380952</v>
+        <v>0.527777777777778</v>
       </c>
       <c r="S78" t="n">
         <v>0.0239441930618401</v>
@@ -5820,16 +5735,15 @@
         <v>0.347435897435897</v>
       </c>
       <c r="V78" t="n">
-        <v>0.016304347826087</v>
+        <v>0.272727272727273</v>
       </c>
       <c r="W78"/>
       <c r="X78"/>
       <c r="Y78"/>
-      <c r="Z78"/>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B79" t="n">
         <v>0.119813406400178</v>
@@ -5861,7 +5775,7 @@
         <v>0.257726269315673</v>
       </c>
       <c r="M79" t="n">
-        <v>0.485715684834239</v>
+        <v>0.48333234941063</v>
       </c>
       <c r="N79" t="n">
         <v>0.25</v>
@@ -5876,7 +5790,7 @@
         <v>0.2</v>
       </c>
       <c r="R79" t="n">
-        <v>0.349206349206349</v>
+        <v>0.407407407407407</v>
       </c>
       <c r="S79" t="n">
         <v>0.0271493212669683</v>
@@ -5891,11 +5805,10 @@
       <c r="W79"/>
       <c r="X79"/>
       <c r="Y79"/>
-      <c r="Z79"/>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B80" t="n">
         <v>0.153325138920898</v>
@@ -5931,7 +5844,7 @@
         <v>0.227373068432671</v>
       </c>
       <c r="M80" t="n">
-        <v>0.652357866901719</v>
+        <v>0.650746797331602</v>
       </c>
       <c r="N80" t="n">
         <v>0.291666666666667</v>
@@ -5946,7 +5859,7 @@
         <v>0.0666666666666667</v>
       </c>
       <c r="R80" t="n">
-        <v>0.468253968253968</v>
+        <v>0.546296296296296</v>
       </c>
       <c r="S80" t="n">
         <v>0.0360105580693816</v>
@@ -5958,16 +5871,15 @@
         <v>0.698717948717949</v>
       </c>
       <c r="V80" t="n">
-        <v>0.0217391304347826</v>
+        <v>0.363636363636364</v>
       </c>
       <c r="W80"/>
       <c r="X80"/>
       <c r="Y80"/>
-      <c r="Z80"/>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B81" t="n">
         <v>0.134759673247804</v>
@@ -6001,7 +5913,7 @@
         <v>0.213300220750552</v>
       </c>
       <c r="M81" t="n">
-        <v>0.490436315557514</v>
+        <v>0.488074856839247</v>
       </c>
       <c r="N81" t="n">
         <v>0.291666666666667</v>
@@ -6014,7 +5926,7 @@
       </c>
       <c r="Q81"/>
       <c r="R81" t="n">
-        <v>0.373015873015873</v>
+        <v>0.435185185185185</v>
       </c>
       <c r="S81" t="n">
         <v>0.0352564102564103</v>
@@ -6029,11 +5941,10 @@
       <c r="W81"/>
       <c r="X81"/>
       <c r="Y81"/>
-      <c r="Z81"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B82" t="n">
         <v>0.0966513875018139</v>
@@ -6067,7 +5978,7 @@
         <v>0.317604856512141</v>
       </c>
       <c r="M82" t="n">
-        <v>0.494784780373145</v>
+        <v>0.492443473640711</v>
       </c>
       <c r="N82" t="n">
         <v>0.40625</v>
@@ -6080,7 +5991,7 @@
       </c>
       <c r="Q82"/>
       <c r="R82" t="n">
-        <v>0.404761904761905</v>
+        <v>0.472222222222222</v>
       </c>
       <c r="S82" t="n">
         <v>0.0316742081447964</v>
@@ -6092,16 +6003,15 @@
         <v>0.588461538461538</v>
       </c>
       <c r="V82" t="n">
-        <v>0.0199275362318841</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="W82"/>
       <c r="X82"/>
       <c r="Y82"/>
-      <c r="Z82"/>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B83" t="n">
         <v>0.182206174831204</v>
@@ -6137,7 +6047,7 @@
         <v>0.217991169977925</v>
       </c>
       <c r="M83" t="n">
-        <v>0.502042015572205</v>
+        <v>0.499734340870181</v>
       </c>
       <c r="N83" t="n">
         <v>0.28125</v>
@@ -6152,7 +6062,7 @@
         <v>0.0666666666666667</v>
       </c>
       <c r="R83" t="n">
-        <v>0.396825396825397</v>
+        <v>0.462962962962963</v>
       </c>
       <c r="S83" t="n">
         <v>0.0361990950226244</v>
@@ -6164,632 +6074,558 @@
         <v>0.698717948717949</v>
       </c>
       <c r="V83" t="n">
-        <v>0.0199275362318841</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="W83"/>
       <c r="X83"/>
       <c r="Y83"/>
-      <c r="Z83"/>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B84" t="n">
-        <v>0.625195257483803</v>
+        <v>0.451311532781918</v>
       </c>
       <c r="C84" t="n">
-        <v>0.164558642603624</v>
+        <v>0.0813647132408694</v>
       </c>
       <c r="D84" t="n">
-        <v>0.0262851773969845</v>
+        <v>0.0277255802623795</v>
       </c>
       <c r="E84" t="n">
-        <v>0.495864513588027</v>
+        <v>0.268767231193383</v>
       </c>
       <c r="F84" t="n">
-        <v>0.117142563681183</v>
+        <v>0.128201177759518</v>
       </c>
       <c r="G84" t="n">
-        <v>0.204295442640126</v>
+        <v>0.158983761131482</v>
       </c>
       <c r="H84"/>
       <c r="I84" t="n">
-        <v>0.962252043795061</v>
+        <v>0.606562746615383</v>
       </c>
       <c r="J84" t="n">
-        <v>0.0747616658304064</v>
-      </c>
-      <c r="K84" t="n">
-        <v>0.0619834710743802</v>
-      </c>
+        <v>0.0605452416792106</v>
+      </c>
+      <c r="K84"/>
       <c r="L84" t="n">
-        <v>0.0322847682119205</v>
+        <v>0.0146247240618102</v>
       </c>
       <c r="M84" t="n">
-        <v>0.0806228882033201</v>
+        <v>0.0781431410748372</v>
       </c>
       <c r="N84"/>
       <c r="O84" t="n">
-        <v>0.293577981651376</v>
+        <v>0.250764525993884</v>
       </c>
       <c r="P84" t="n">
-        <v>0.027027027027027</v>
+        <v>0.0630630630630631</v>
       </c>
       <c r="Q84"/>
       <c r="R84" t="n">
-        <v>0.0952380952380952</v>
+        <v>0.157407407407407</v>
       </c>
       <c r="S84" t="n">
-        <v>0.427601809954751</v>
+        <v>0.402714932126697</v>
       </c>
       <c r="T84"/>
       <c r="U84" t="n">
-        <v>0.157692307692308</v>
+        <v>0.125641025641026</v>
       </c>
       <c r="V84"/>
       <c r="W84"/>
-      <c r="X84" t="n">
-        <v>0.0543478260869564</v>
-      </c>
+      <c r="X84"/>
       <c r="Y84"/>
-      <c r="Z84"/>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B85" t="n">
-        <v>0.451311532781918</v>
+        <v>0.566421687878245</v>
       </c>
       <c r="C85" t="n">
-        <v>0.0813647132408694</v>
+        <v>0.125360311320783</v>
       </c>
       <c r="D85" t="n">
-        <v>0.0277255802623795</v>
+        <v>0.0755571463369772</v>
       </c>
       <c r="E85" t="n">
-        <v>0.268767231193383</v>
+        <v>0.447131416568203</v>
       </c>
       <c r="F85" t="n">
-        <v>0.128201177759518</v>
+        <v>0.17909476855656</v>
       </c>
       <c r="G85" t="n">
-        <v>0.158983761131482</v>
+        <v>0.119172341540073</v>
       </c>
       <c r="H85"/>
       <c r="I85" t="n">
-        <v>0.606562746615383</v>
+        <v>0.653327408179267</v>
       </c>
       <c r="J85" t="n">
-        <v>0.0605452416792106</v>
+        <v>0.0895355968110609</v>
       </c>
       <c r="K85"/>
       <c r="L85" t="n">
-        <v>0.0146247240618102</v>
+        <v>0.0328366445916115</v>
       </c>
       <c r="M85" t="n">
-        <v>0.082395573184467</v>
+        <v>0.0855127221205502</v>
       </c>
       <c r="N85"/>
       <c r="O85" t="n">
-        <v>0.250764525993884</v>
+        <v>0.27217125382263</v>
       </c>
       <c r="P85" t="n">
-        <v>0.0630630630630631</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="Q85"/>
-      <c r="R85" t="n">
-        <v>0.134920634920635</v>
-      </c>
+      <c r="R85"/>
       <c r="S85" t="n">
-        <v>0.402714932126697</v>
+        <v>0.307126696832579</v>
       </c>
       <c r="T85"/>
       <c r="U85" t="n">
-        <v>0.125641025641026</v>
+        <v>0.0576923076923077</v>
       </c>
       <c r="V85"/>
       <c r="W85"/>
       <c r="X85"/>
       <c r="Y85"/>
-      <c r="Z85"/>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B86" t="n">
-        <v>0.566421687878245</v>
+        <v>0.576728722269169</v>
       </c>
       <c r="C86" t="n">
-        <v>0.125360311320783</v>
-      </c>
-      <c r="D86" t="n">
-        <v>0.0755571463369772</v>
-      </c>
+        <v>0.0948743594055638</v>
+      </c>
+      <c r="D86"/>
       <c r="E86" t="n">
-        <v>0.447131416568203</v>
+        <v>0.422318498096363</v>
       </c>
       <c r="F86" t="n">
-        <v>0.17909476855656</v>
+        <v>0.0901978909887702</v>
       </c>
       <c r="G86" t="n">
-        <v>0.119172341540073</v>
+        <v>0.167888947092719</v>
       </c>
       <c r="H86"/>
       <c r="I86" t="n">
-        <v>0.653327408179267</v>
+        <v>0.908831799688929</v>
       </c>
       <c r="J86" t="n">
-        <v>0.0895355968110609</v>
+        <v>0.0219657690806712</v>
       </c>
       <c r="K86"/>
       <c r="L86" t="n">
-        <v>0.0328366445916115</v>
+        <v>0.0242825607064018</v>
       </c>
       <c r="M86" t="n">
-        <v>0.0897311591009255</v>
+        <v>0.116161914320011</v>
       </c>
       <c r="N86"/>
       <c r="O86" t="n">
-        <v>0.27217125382263</v>
+        <v>0.259938837920489</v>
       </c>
       <c r="P86" t="n">
-        <v>0.166666666666667</v>
+        <v>0.045045045045045</v>
       </c>
       <c r="Q86"/>
       <c r="R86"/>
       <c r="S86" t="n">
-        <v>0.307126696832579</v>
+        <v>0.332956259426848</v>
       </c>
       <c r="T86"/>
       <c r="U86" t="n">
-        <v>0.0576923076923077</v>
+        <v>0.0551282051282051</v>
       </c>
       <c r="V86"/>
       <c r="W86"/>
       <c r="X86"/>
       <c r="Y86"/>
-      <c r="Z86"/>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B87" t="n">
-        <v>0.576728722269169</v>
+        <v>0.80193849069166</v>
       </c>
       <c r="C87" t="n">
-        <v>0.0948743594055638</v>
-      </c>
-      <c r="D87"/>
+        <v>0.346751518691933</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.38637408716488</v>
+      </c>
       <c r="E87" t="n">
-        <v>0.422318498096363</v>
+        <v>0.861310227123539</v>
       </c>
       <c r="F87" t="n">
-        <v>0.0901978909887702</v>
+        <v>0.860123938646946</v>
       </c>
       <c r="G87" t="n">
-        <v>0.167888947092719</v>
-      </c>
-      <c r="H87"/>
+        <v>0.170857342413131</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.664253418767857</v>
+      </c>
       <c r="I87" t="n">
-        <v>0.908831799688929</v>
+        <v>0.502260880447247</v>
       </c>
       <c r="J87" t="n">
-        <v>0.0219657690806712</v>
+        <v>0.410771031945141</v>
       </c>
       <c r="K87"/>
       <c r="L87" t="n">
-        <v>0.0242825607064018</v>
+        <v>0.180739514348786</v>
       </c>
       <c r="M87" t="n">
-        <v>0.120238969688066</v>
+        <v>0.478009327587225</v>
       </c>
       <c r="N87"/>
       <c r="O87" t="n">
-        <v>0.259938837920489</v>
+        <v>0.357798165137615</v>
       </c>
       <c r="P87" t="n">
-        <v>0.045045045045045</v>
+        <v>0.689189189189189</v>
       </c>
       <c r="Q87"/>
-      <c r="R87"/>
+      <c r="R87" t="n">
+        <v>0.453703703703704</v>
+      </c>
       <c r="S87" t="n">
-        <v>0.332956259426848</v>
-      </c>
-      <c r="T87"/>
+        <v>0.26263197586727</v>
+      </c>
+      <c r="T87" t="n">
+        <v>0.2</v>
+      </c>
       <c r="U87" t="n">
-        <v>0.0551282051282051</v>
+        <v>0.284615384615385</v>
       </c>
       <c r="V87"/>
-      <c r="W87"/>
+      <c r="W87" t="n">
+        <v>0.412698412698413</v>
+      </c>
       <c r="X87"/>
       <c r="Y87"/>
-      <c r="Z87"/>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B88" t="n">
-        <v>0.80193849069166</v>
+        <v>0.702222734372999</v>
       </c>
       <c r="C88" t="n">
-        <v>0.346751518691933</v>
+        <v>0.403648991128302</v>
       </c>
       <c r="D88" t="n">
-        <v>0.38637408716488</v>
+        <v>0.408590965355763</v>
       </c>
       <c r="E88" t="n">
-        <v>0.861310227123539</v>
+        <v>0.814257581725089</v>
       </c>
       <c r="F88" t="n">
-        <v>0.860123938646946</v>
+        <v>0.554676800876472</v>
       </c>
       <c r="G88" t="n">
-        <v>0.170857342413131</v>
+        <v>0.110354461323555</v>
       </c>
       <c r="H88" t="n">
-        <v>0.664253418767857</v>
+        <v>0.726193448170647</v>
       </c>
       <c r="I88" t="n">
-        <v>0.502260880447247</v>
+        <v>0.475457220132243</v>
       </c>
       <c r="J88" t="n">
-        <v>0.410771031945141</v>
+        <v>0.469364999721247</v>
       </c>
       <c r="K88"/>
       <c r="L88" t="n">
-        <v>0.180739514348786</v>
+        <v>0.231512141280353</v>
       </c>
       <c r="M88" t="n">
-        <v>0.480417217570148</v>
-      </c>
-      <c r="N88"/>
+        <v>0.570842434618336</v>
+      </c>
+      <c r="N88" t="n">
+        <v>0.354166666666667</v>
+      </c>
       <c r="O88" t="n">
-        <v>0.357798165137615</v>
+        <v>0.409785932721713</v>
       </c>
       <c r="P88" t="n">
-        <v>0.689189189189189</v>
+        <v>0.684684684684685</v>
       </c>
       <c r="Q88"/>
       <c r="R88" t="n">
-        <v>0.388888888888889</v>
+        <v>0.537037037037037</v>
       </c>
       <c r="S88" t="n">
-        <v>0.26263197586727</v>
+        <v>0.2526395173454</v>
       </c>
       <c r="T88" t="n">
-        <v>0.2</v>
+        <v>0.346666666666667</v>
       </c>
       <c r="U88" t="n">
-        <v>0.284615384615385</v>
-      </c>
-      <c r="V88"/>
-      <c r="W88" t="n">
-        <v>0.0337224383916991</v>
-      </c>
+        <v>0.314102564102564</v>
+      </c>
+      <c r="V88" t="n">
+        <v>0.454545454545455</v>
+      </c>
+      <c r="W88"/>
       <c r="X88"/>
       <c r="Y88"/>
-      <c r="Z88"/>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B89" t="n">
-        <v>0.702222734372999</v>
+        <v>0.521561547719649</v>
       </c>
       <c r="C89" t="n">
-        <v>0.403648991128302</v>
+        <v>0.270791844056375</v>
       </c>
       <c r="D89" t="n">
-        <v>0.408590965355763</v>
+        <v>0.222334695439926</v>
       </c>
       <c r="E89" t="n">
-        <v>0.814257581725089</v>
+        <v>0.314480766706052</v>
       </c>
       <c r="F89" t="n">
-        <v>0.554676800876472</v>
+        <v>0.359422076143522</v>
       </c>
       <c r="G89" t="n">
-        <v>0.110354461323555</v>
+        <v>0.319277108433735</v>
       </c>
       <c r="H89" t="n">
-        <v>0.726193448170647</v>
+        <v>0.356633657873568</v>
       </c>
       <c r="I89" t="n">
-        <v>0.475457220132243</v>
+        <v>0.537878845923009</v>
       </c>
       <c r="J89" t="n">
-        <v>0.469364999721247</v>
+        <v>0.395216591403245</v>
       </c>
       <c r="K89"/>
       <c r="L89" t="n">
-        <v>0.231512141280353</v>
+        <v>0.070364238410596</v>
       </c>
       <c r="M89" t="n">
-        <v>0.572822094902306</v>
-      </c>
-      <c r="N89" t="n">
-        <v>0.354166666666667</v>
-      </c>
+        <v>0.329358285613082</v>
+      </c>
+      <c r="N89"/>
       <c r="O89" t="n">
-        <v>0.409785932721713</v>
+        <v>0.201834862385321</v>
       </c>
       <c r="P89" t="n">
-        <v>0.684684684684685</v>
+        <v>0.297297297297297</v>
       </c>
       <c r="Q89"/>
       <c r="R89" t="n">
-        <v>0.46031746031746</v>
+        <v>0.361111111111111</v>
       </c>
       <c r="S89" t="n">
-        <v>0.2526395173454</v>
-      </c>
-      <c r="T89" t="n">
-        <v>0.346666666666667</v>
-      </c>
+        <v>0.218325791855204</v>
+      </c>
+      <c r="T89"/>
       <c r="U89" t="n">
-        <v>0.314102564102564</v>
-      </c>
-      <c r="V89" t="n">
-        <v>0.0271739130434783</v>
-      </c>
+        <v>0.220512820512821</v>
+      </c>
+      <c r="V89"/>
       <c r="W89"/>
       <c r="X89"/>
       <c r="Y89"/>
-      <c r="Z89"/>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B90" t="n">
-        <v>0.521561547719649</v>
+        <v>0.432703387877391</v>
       </c>
       <c r="C90" t="n">
-        <v>0.270791844056375</v>
+        <v>0.110227973435061</v>
       </c>
       <c r="D90" t="n">
-        <v>0.222334695439926</v>
+        <v>0.301877494916956</v>
       </c>
       <c r="E90" t="n">
-        <v>0.314480766706052</v>
+        <v>0.2855980044637</v>
       </c>
       <c r="F90" t="n">
-        <v>0.359422076143522</v>
+        <v>0.129519309778143</v>
       </c>
       <c r="G90" t="n">
-        <v>0.319277108433735</v>
-      </c>
-      <c r="H90" t="n">
-        <v>0.356633657873568</v>
-      </c>
+        <v>0.176619521564519</v>
+      </c>
+      <c r="H90"/>
       <c r="I90" t="n">
-        <v>0.537878845923009</v>
+        <v>0.49113908532988</v>
       </c>
       <c r="J90" t="n">
-        <v>0.395216591403245</v>
+        <v>0.133188381557674</v>
       </c>
       <c r="K90"/>
       <c r="L90" t="n">
-        <v>0.070364238410596</v>
+        <v>0.0303532008830022</v>
       </c>
       <c r="M90" t="n">
-        <v>0.332451887762597</v>
+        <v>0.0909439754412893</v>
       </c>
       <c r="N90"/>
       <c r="O90" t="n">
-        <v>0.201834862385321</v>
+        <v>0.262996941896024</v>
       </c>
       <c r="P90" t="n">
-        <v>0.297297297297297</v>
+        <v>0.202702702702703</v>
       </c>
       <c r="Q90"/>
-      <c r="R90" t="n">
-        <v>0.309523809523809</v>
-      </c>
+      <c r="R90"/>
       <c r="S90" t="n">
-        <v>0.218325791855204</v>
+        <v>0.455693815987934</v>
       </c>
       <c r="T90"/>
       <c r="U90" t="n">
-        <v>0.220512820512821</v>
+        <v>0.148717948717949</v>
       </c>
       <c r="V90"/>
       <c r="W90"/>
       <c r="X90"/>
       <c r="Y90"/>
-      <c r="Z90"/>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B91" t="n">
-        <v>0.432703387877391</v>
+        <v>0.389260198202351</v>
       </c>
       <c r="C91" t="n">
-        <v>0.110227973435061</v>
+        <v>0.214711618177688</v>
       </c>
       <c r="D91" t="n">
-        <v>0.301877494916956</v>
+        <v>0.319172893084575</v>
       </c>
       <c r="E91" t="n">
-        <v>0.2855980044637</v>
+        <v>0.673913614283839</v>
       </c>
       <c r="F91" t="n">
-        <v>0.129519309778143</v>
+        <v>0.075955217748562</v>
       </c>
       <c r="G91" t="n">
-        <v>0.176619521564519</v>
-      </c>
-      <c r="H91"/>
+        <v>0.149205517723066</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.47629746747663</v>
+      </c>
       <c r="I91" t="n">
-        <v>0.49113908532988</v>
+        <v>0.461330069390705</v>
       </c>
       <c r="J91" t="n">
-        <v>0.133188381557674</v>
+        <v>0.311702068350337</v>
       </c>
       <c r="K91"/>
       <c r="L91" t="n">
-        <v>0.0303532008830022</v>
+        <v>0.0943708609271523</v>
       </c>
       <c r="M91" t="n">
-        <v>0.0951373586014397</v>
+        <v>0.263287876104453</v>
       </c>
       <c r="N91"/>
       <c r="O91" t="n">
-        <v>0.262996941896024</v>
+        <v>0.27217125382263</v>
       </c>
       <c r="P91" t="n">
-        <v>0.202702702702703</v>
+        <v>0.495495495495495</v>
       </c>
       <c r="Q91"/>
-      <c r="R91"/>
+      <c r="R91" t="n">
+        <v>0.305555555555556</v>
+      </c>
       <c r="S91" t="n">
-        <v>0.455693815987934</v>
+        <v>0.28393665158371</v>
       </c>
       <c r="T91"/>
       <c r="U91" t="n">
-        <v>0.148717948717949</v>
+        <v>0.191025641025641</v>
       </c>
       <c r="V91"/>
       <c r="W91"/>
-      <c r="X91"/>
+      <c r="X91" t="n">
+        <v>0.214731585518102</v>
+      </c>
       <c r="Y91"/>
-      <c r="Z91"/>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B92" t="n">
-        <v>0.389260198202351</v>
+        <v>0.511096600172424</v>
       </c>
       <c r="C92" t="n">
-        <v>0.214711618177688</v>
+        <v>0.251478862227572</v>
       </c>
       <c r="D92" t="n">
-        <v>0.319172893084575</v>
+        <v>0.322758986672234</v>
       </c>
       <c r="E92" t="n">
-        <v>0.673913614283839</v>
+        <v>0.595720099776815</v>
       </c>
       <c r="F92" t="n">
-        <v>0.075955217748562</v>
+        <v>0.249811695425911</v>
       </c>
       <c r="G92" t="n">
-        <v>0.149205517723066</v>
+        <v>0.953727955299459</v>
       </c>
       <c r="H92" t="n">
-        <v>0.47629746747663</v>
+        <v>0.572272613797121</v>
       </c>
       <c r="I92" t="n">
-        <v>0.461330069390705</v>
+        <v>0.461489052511678</v>
       </c>
       <c r="J92" t="n">
-        <v>0.311702068350337</v>
+        <v>0.307130512348776</v>
       </c>
       <c r="K92"/>
       <c r="L92" t="n">
-        <v>0.0943708609271523</v>
+        <v>0.162251655629139</v>
       </c>
       <c r="M92" t="n">
-        <v>0.266686254346016</v>
-      </c>
-      <c r="N92"/>
+        <v>0.365133715095342</v>
+      </c>
+      <c r="N92" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="O92" t="n">
         <v>0.27217125382263</v>
       </c>
       <c r="P92" t="n">
-        <v>0.495495495495495</v>
+        <v>0.657657657657658</v>
       </c>
       <c r="Q92"/>
       <c r="R92" t="n">
-        <v>0.261904761904762</v>
+        <v>0.453703703703704</v>
       </c>
       <c r="S92" t="n">
-        <v>0.28393665158371</v>
+        <v>0.283748114630468</v>
       </c>
       <c r="T92"/>
       <c r="U92" t="n">
-        <v>0.191025641025641</v>
+        <v>0.247435897435897</v>
       </c>
       <c r="V92"/>
       <c r="W92"/>
       <c r="X92"/>
-      <c r="Y92" t="n">
-        <v>0.0800744878957169</v>
-      </c>
-      <c r="Z92"/>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>117</v>
-      </c>
-      <c r="B93" t="n">
-        <v>0.511096600172424</v>
-      </c>
-      <c r="C93" t="n">
-        <v>0.251478862227572</v>
-      </c>
-      <c r="D93" t="n">
-        <v>0.322758986672234</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0.595720099776815</v>
-      </c>
-      <c r="F93" t="n">
-        <v>0.249811695425911</v>
-      </c>
-      <c r="G93" t="n">
-        <v>0.953727955299459</v>
-      </c>
-      <c r="H93" t="n">
-        <v>0.572272613797121</v>
-      </c>
-      <c r="I93" t="n">
-        <v>0.461489052511678</v>
-      </c>
-      <c r="J93" t="n">
-        <v>0.307130512348776</v>
-      </c>
-      <c r="K93"/>
-      <c r="L93" t="n">
-        <v>0.162251655629139</v>
-      </c>
-      <c r="M93" t="n">
-        <v>0.368062288820332</v>
-      </c>
-      <c r="N93" t="n">
-        <v>0.1875</v>
-      </c>
-      <c r="O93" t="n">
-        <v>0.27217125382263</v>
-      </c>
-      <c r="P93" t="n">
-        <v>0.657657657657658</v>
-      </c>
-      <c r="Q93"/>
-      <c r="R93" t="n">
-        <v>0.388888888888889</v>
-      </c>
-      <c r="S93" t="n">
-        <v>0.283748114630468</v>
-      </c>
-      <c r="T93"/>
-      <c r="U93" t="n">
-        <v>0.247435897435897</v>
-      </c>
-      <c r="V93"/>
-      <c r="W93"/>
-      <c r="X93"/>
-      <c r="Y93"/>
-      <c r="Z93"/>
+      <c r="Y92"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>